<commit_message>
Copy Files From Source Repo (2025-03-19 22:06)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <r>
       <rPr>
@@ -129,6 +129,17 @@
         <family val="2"/>
       </rPr>
       <t>4:36</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>5:48</t>
     </r>
   </si>
   <si>
@@ -887,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>2996</v>
@@ -904,8 +915,8 @@
       <c r="C7">
         <v>315</v>
       </c>
-      <c r="D7">
-        <v>548</v>
+      <c r="D7" t="s">
+        <v>8</v>
       </c>
       <c r="E7">
         <v>3599</v>

</xml_diff>